<commit_message>
[rps update] forgot to save the excel file before the commit.
</commit_message>
<xml_diff>
--- a/rps_update/rps_updates.xlsx
+++ b/rps_update/rps_updates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="32100" yWindow="560" windowWidth="14180" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="24660" yWindow="2740" windowWidth="26200" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>CA</t>
+  </si>
+  <si>
+    <t>OR_E</t>
+  </si>
+  <si>
+    <t>OR_PDX</t>
+  </si>
+  <si>
+    <t>OR_W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -73,7 +85,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -111,11 +123,146 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="171">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -134,6 +281,73 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -152,6 +366,73 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -427,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -551,8 +832,342 @@
         <v>0.50000000000000011</v>
       </c>
     </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>2025</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.25557800000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17">
+        <f>B16+1</f>
+        <v>2026</v>
+      </c>
+      <c r="C17" s="1">
+        <f>C16+A$18</f>
+        <v>0.27187280000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <f>(C31-C16)/15</f>
+        <v>1.6294799999999998E-2</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ref="B18:B31" si="2">B17+1</f>
+        <v>2027</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:C30" si="3">C17+A$18</f>
+        <v>0.28816760000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>2028</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="3"/>
+        <v>0.30446240000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>2029</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="3"/>
+        <v>0.32075720000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>2030</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="3"/>
+        <v>0.33705200000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>2031</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="3"/>
+        <v>0.35334680000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>2032</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="3"/>
+        <v>0.36964160000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24">
+        <f t="shared" si="2"/>
+        <v>2033</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="3"/>
+        <v>0.38593640000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25">
+        <f t="shared" si="2"/>
+        <v>2034</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="3"/>
+        <v>0.40223120000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26">
+        <f t="shared" si="2"/>
+        <v>2035</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="3"/>
+        <v>0.41852600000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27">
+        <f t="shared" si="2"/>
+        <v>2036</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="3"/>
+        <v>0.43482080000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28">
+        <f t="shared" si="2"/>
+        <v>2037</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="3"/>
+        <v>0.45111560000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29">
+        <f t="shared" si="2"/>
+        <v>2038</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="3"/>
+        <v>0.4674104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30">
+        <f t="shared" si="2"/>
+        <v>2039</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="3"/>
+        <v>0.4837052</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31">
+        <f t="shared" si="2"/>
+        <v>2040</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>2025</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.231989</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35">
+        <f>B34+1</f>
+        <v>2026</v>
+      </c>
+      <c r="C35" s="1">
+        <f>C34+$A$36</f>
+        <v>0.24985640000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <f>(C49-C34)/15</f>
+        <v>1.7867399999999999E-2</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ref="B36:B49" si="4">B35+1</f>
+        <v>2027</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" ref="C36:C48" si="5">C35+$A$36</f>
+        <v>0.26772380000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37">
+        <f t="shared" si="4"/>
+        <v>2028</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="5"/>
+        <v>0.28559119999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38">
+        <f t="shared" si="4"/>
+        <v>2029</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="5"/>
+        <v>0.30345859999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39">
+        <f t="shared" si="4"/>
+        <v>2030</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="5"/>
+        <v>0.32132599999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40">
+        <f t="shared" si="4"/>
+        <v>2031</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="5"/>
+        <v>0.33919339999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41">
+        <f t="shared" si="4"/>
+        <v>2032</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="5"/>
+        <v>0.3570607999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42">
+        <f t="shared" si="4"/>
+        <v>2033</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="5"/>
+        <v>0.37492819999999988</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43">
+        <f t="shared" si="4"/>
+        <v>2034</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="5"/>
+        <v>0.39279559999999986</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44">
+        <f t="shared" si="4"/>
+        <v>2035</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="5"/>
+        <v>0.41066299999999983</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45">
+        <f t="shared" si="4"/>
+        <v>2036</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="5"/>
+        <v>0.42853039999999981</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46">
+        <f t="shared" si="4"/>
+        <v>2037</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="5"/>
+        <v>0.44639779999999979</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47">
+        <f t="shared" si="4"/>
+        <v>2038</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="5"/>
+        <v>0.46426519999999977</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48">
+        <f t="shared" si="4"/>
+        <v>2039</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="5"/>
+        <v>0.48213259999999974</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49">
+        <f t="shared" si="4"/>
+        <v>2040</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>